<commit_message>
wip(writing): added evaluation chapter text
</commit_message>
<xml_diff>
--- a/evaluation/use case 3/temperature-usecase.xlsx
+++ b/evaluation/use case 3/temperature-usecase.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="temp (8)" sheetId="12" r:id="rId1"/>
-    <sheet name="temp (7)" sheetId="11" r:id="rId2"/>
-    <sheet name="temp (6)" sheetId="10" r:id="rId3"/>
-    <sheet name="temp (5)" sheetId="9" r:id="rId4"/>
-    <sheet name="temp (4)" sheetId="8" r:id="rId5"/>
-    <sheet name="temp (3)" sheetId="7" r:id="rId6"/>
-    <sheet name="temp (2)" sheetId="6" r:id="rId7"/>
-    <sheet name="temp" sheetId="1" r:id="rId8"/>
+    <sheet name="results" sheetId="14" r:id="rId2"/>
+    <sheet name="temp (7)" sheetId="11" r:id="rId3"/>
+    <sheet name="temp (6)" sheetId="10" r:id="rId4"/>
+    <sheet name="temp (5)" sheetId="9" r:id="rId5"/>
+    <sheet name="temp (4)" sheetId="8" r:id="rId6"/>
+    <sheet name="temp (3)" sheetId="7" r:id="rId7"/>
+    <sheet name="temp (2)" sheetId="6" r:id="rId8"/>
+    <sheet name="temp" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
   <si>
     <t>pi</t>
   </si>
@@ -168,6 +169,21 @@
   </si>
   <si>
     <t>29 May 13:49:42 - [info] [function:adjust] Mon May 29 2017 13:49:42 GMT+0200 (CEST):569 , Adding to temp27.437</t>
+  </si>
+  <si>
+    <t>pc-&gt;pi</t>
+  </si>
+  <si>
+    <t>time to first db insert</t>
+  </si>
+  <si>
+    <t>pc-&gt;p2</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>std</t>
   </si>
 </sst>
 </file>
@@ -488,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,6 +648,235 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4.5419999999999998</v>
+      </c>
+      <c r="C2">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="D2">
+        <v>4.6929999999999996</v>
+      </c>
+      <c r="E2">
+        <v>1.726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.4380000000000002</v>
+      </c>
+      <c r="C3">
+        <v>1.706</v>
+      </c>
+      <c r="D3">
+        <v>2.5329999999999999</v>
+      </c>
+      <c r="E3">
+        <v>1.716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.8849999999999998</v>
+      </c>
+      <c r="C4">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="D4">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="E4">
+        <v>1.7170000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.4510000000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="D5">
+        <v>2.4620000000000002</v>
+      </c>
+      <c r="E5">
+        <v>1.7230000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="C6">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.536</v>
+      </c>
+      <c r="E6">
+        <v>1.6850000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2.423</v>
+      </c>
+      <c r="C7">
+        <v>1.724</v>
+      </c>
+      <c r="D7">
+        <v>1.444</v>
+      </c>
+      <c r="E7">
+        <v>1.7270000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3.4369999999999998</v>
+      </c>
+      <c r="C8">
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="D8">
+        <v>2.4140000000000001</v>
+      </c>
+      <c r="E8">
+        <v>1.722</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="C9">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="D9">
+        <v>2.35</v>
+      </c>
+      <c r="E9">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B9)</f>
+        <v>2.8702500000000004</v>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(C2:C9)</f>
+        <v>1.7235</v>
+      </c>
+      <c r="D10">
+        <f>AVERAGE(D2:D9)</f>
+        <v>2.437125</v>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(E2:E9)</f>
+        <v>1.7170000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <f>STDEV(B2:B9)</f>
+        <v>0.76918783698874482</v>
+      </c>
+      <c r="C11">
+        <f>STDEV(C2:C9)</f>
+        <v>3.7614586836188166E-2</v>
+      </c>
+      <c r="D11">
+        <f>STDEV(D2:D9)</f>
+        <v>1.0031172040195497</v>
+      </c>
+      <c r="E11">
+        <f>STDEV(E2:E9)</f>
+        <v>1.3501322686526462E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f xml:space="preserve"> AVERAGE(B10,D10)</f>
+        <v>2.6536875000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f>AVERAGE(C10,E10)</f>
+        <v>1.7202500000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f>B15+B16</f>
+        <v>4.3739375000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -780,7 +1025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -927,12 +1172,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B32" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1076,12 +1321,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,7 +1468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -1374,7 +1619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -1521,12 +1766,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>